<commit_message>
had to go back a few steps to better format my code
</commit_message>
<xml_diff>
--- a/MockDatabase.xlsx
+++ b/MockDatabase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="69">
   <si>
     <t>Station Name</t>
   </si>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1001,14 +1001,435 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A13:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="1">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1854</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="1">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1852</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="1">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1842</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="1">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1846</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1850</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="1">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1879</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="1">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1836</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="1">
+        <v>17</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1938</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="1">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1840</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="1">
+        <v>12</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1850</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1870</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="1">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1839</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1852</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1839</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="1">
+        <v>5</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1845</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1841</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="1">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1848</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1850</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1876</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="1">
+        <v>6</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1840</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>